<commit_message>
Added meta info to all. Consolidated menus. Added all about info.
</commit_message>
<xml_diff>
--- a/misc/Volunteer Information ('19_'20).xlsx
+++ b/misc/Volunteer Information ('19_'20).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aqila/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISVir\OneDrive\Desktop\AMCRT\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC1AFF1-73A7-CB4B-B68B-014DF342EBC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14970" yWindow="-90" windowWidth="20560" windowHeight="10580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,16 +506,16 @@
   <dimension ref="A3:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="37.5" customWidth="1"/>
+    <col min="1" max="1" width="29.81640625" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="14">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>